<commit_message>
Forming up Beijing Environmental table
</commit_message>
<xml_diff>
--- a/viz/Beijing_Neighbors.xlsx
+++ b/viz/Beijing_Neighbors.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21070" windowHeight="13010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21070" windowHeight="13010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beijing_Nearest_Neighbor" sheetId="2" r:id="rId1"/>
-    <sheet name="Beijing_1ring_Neighbors" sheetId="1" r:id="rId2"/>
+    <sheet name="Beijing_Enviornment" sheetId="3" r:id="rId2"/>
+    <sheet name="Beijing_1ring_Neighbors" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Beijing_1ring_Neighbors!$A$1:$F$725</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Beijing_1ring_Neighbors!$A$1:$F$725</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Beijing_Enviornment!$A$1:$H$659</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Beijing_Nearest_Neighbor!$A$1:$B$709</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
   <si>
     <t>shunyi_meo</t>
   </si>
@@ -303,6 +305,12 @@
   </si>
   <si>
     <t>fangshan_met</t>
+  </si>
+  <si>
+    <t>station_id</t>
+  </si>
+  <si>
+    <t>landclass</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="A1:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1452,10 +1460,253 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="20.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F725"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2061,6 +2312,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F725"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Got env. data for Beijing
</commit_message>
<xml_diff>
--- a/viz/Beijing_Neighbors.xlsx
+++ b/viz/Beijing_Neighbors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21070" windowHeight="13010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21069" windowHeight="13011" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beijing_Nearest_Neighbor" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Beijing_1ring_Neighbors!$A$1:$F$725</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Beijing_Enviornment!$A$1:$H$639</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Beijing_Enviornment!$A$1:$H$637</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Beijing_Nearest_Neighbor!$A$1:$B$709</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="98">
   <si>
     <t>shunyi_meo</t>
   </si>
@@ -304,13 +304,22 @@
     <t>W</t>
   </si>
   <si>
-    <t>fangshan_met</t>
-  </si>
-  <si>
     <t>station_id</t>
   </si>
   <si>
     <t>landclass</t>
+  </si>
+  <si>
+    <t>orchard</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>reservoir</t>
+  </si>
+  <si>
+    <t>fangshan_meo</t>
   </si>
 </sst>
 </file>
@@ -635,7 +644,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,8 +809,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1160,16 +1171,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="A1:B36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="20.26953125" customWidth="1"/>
+    <col min="1" max="2" width="20.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -1177,7 +1188,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1185,7 +1196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1193,7 +1204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1201,7 +1212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1209,7 +1220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -1217,7 +1228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1225,7 +1236,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1233,7 +1244,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1241,15 +1252,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1257,7 +1268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1265,7 +1276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1273,7 +1284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1281,7 +1292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -1289,7 +1300,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1297,7 +1308,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1305,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1313,7 +1324,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1321,7 +1332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1329,7 +1340,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1337,7 +1348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1353,7 +1364,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1361,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1369,7 +1380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1377,7 +1388,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1385,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1393,7 +1404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1401,7 +1412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1409,7 +1420,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1417,7 +1428,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1425,7 +1436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -1433,7 +1444,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1441,7 +1452,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -1449,7 +1460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1467,29 +1478,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="4" width="20.26953125" customWidth="1"/>
+    <col min="1" max="1" width="17.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
         <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1500,7 +1514,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1511,7 +1525,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1522,7 +1536,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +1547,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1544,126 +1558,174 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>78</v>
@@ -1672,14 +1734,20 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>78</v>
@@ -1688,9 +1756,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>78</v>
@@ -1699,270 +1767,507 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
         <v>78</v>
       </c>
       <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A63" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B65" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>71</v>
-      </c>
-      <c r="B66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
         <v>40</v>
       </c>
+      <c r="B70" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C72">
-    <sortCondition ref="A2:A72"/>
+  <sortState ref="A2:C70">
+    <sortCondition ref="A2:A70"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1974,14 +2279,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="20.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" customWidth="1"/>
+    <col min="1" max="2" width="20.23046875" customWidth="1"/>
+    <col min="3" max="3" width="14.23046875" customWidth="1"/>
+    <col min="4" max="4" width="19.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2001,27 +2306,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2041,17 +2346,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2071,77 +2376,77 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -2161,12 +2466,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2186,57 +2491,57 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="706" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="706" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A706" t="s">
         <v>54</v>
       </c>
@@ -2256,7 +2561,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="707" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="707" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A707" t="s">
         <v>54</v>
       </c>
@@ -2276,7 +2581,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="708" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="708" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A708" t="s">
         <v>54</v>
       </c>
@@ -2296,7 +2601,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="709" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="709" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A709" t="s">
         <v>54</v>
       </c>
@@ -2316,7 +2621,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="710" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="710" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A710" t="s">
         <v>54</v>
       </c>
@@ -2336,7 +2641,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="711" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="711" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A711" t="s">
         <v>36</v>
       </c>
@@ -2356,7 +2661,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="712" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="712" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A712" t="s">
         <v>36</v>
       </c>
@@ -2376,7 +2681,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="713" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="713" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A713" t="s">
         <v>36</v>
       </c>
@@ -2396,7 +2701,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="714" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="714" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A714" t="s">
         <v>36</v>
       </c>
@@ -2416,7 +2721,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="715" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="715" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A715" t="s">
         <v>56</v>
       </c>
@@ -2436,7 +2741,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="716" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="716" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A716" t="s">
         <v>56</v>
       </c>
@@ -2456,7 +2761,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="717" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="717" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A717" t="s">
         <v>56</v>
       </c>
@@ -2476,7 +2781,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="718" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="718" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A718" t="s">
         <v>56</v>
       </c>
@@ -2496,7 +2801,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="719" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="719" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A719" t="s">
         <v>56</v>
       </c>
@@ -2516,7 +2821,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="720" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="720" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A720" t="s">
         <v>36</v>
       </c>
@@ -2536,7 +2841,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="721" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="721" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A721" t="s">
         <v>36</v>
       </c>
@@ -2556,22 +2861,22 @@
         <v>79</v>
       </c>
     </row>
-    <row r="722" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="722" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A722" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="723" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="723" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A723" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="724" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="724" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A724" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="725" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="725" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A725" t="s">
         <v>39</v>
       </c>

</xml_diff>